<commit_message>
update README and analysis
</commit_message>
<xml_diff>
--- a/analysis/tracks/tracks.xlsx
+++ b/analysis/tracks/tracks.xlsx
@@ -8,21 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicobader/Documents/Uni_Leipzig/master_thesis/analysis/tracks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2E59D80-B7A5-A445-805B-C8907C6E3EFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DE62305-6735-DC4A-9E37-E2A5A05EDB61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19740" yWindow="500" windowWidth="16100" windowHeight="19420" xr2:uid="{CD197590-A4A5-7545-83E8-3495E8E7C9EB}"/>
+    <workbookView xWindow="19740" yWindow="500" windowWidth="16100" windowHeight="19420" activeTab="5" xr2:uid="{CD197590-A4A5-7545-83E8-3495E8E7C9EB}"/>
   </bookViews>
   <sheets>
-    <sheet name="new_2021-06-01" sheetId="10" r:id="rId1"/>
-    <sheet name="new_2021-06-02" sheetId="11" r:id="rId2"/>
+    <sheet name="2021-06-01" sheetId="10" r:id="rId1"/>
+    <sheet name="2021-06-02" sheetId="11" r:id="rId2"/>
     <sheet name="2021-06-04" sheetId="3" r:id="rId3"/>
     <sheet name="2021-06-05" sheetId="4" r:id="rId4"/>
     <sheet name="2021-06-08" sheetId="9" r:id="rId5"/>
-    <sheet name="2021-06-21" sheetId="1" r:id="rId6"/>
-    <sheet name="2021-06-22" sheetId="2" r:id="rId7"/>
-    <sheet name="2021-07-13" sheetId="6" r:id="rId8"/>
-    <sheet name="2021-07-25" sheetId="7" r:id="rId9"/>
-    <sheet name="2021-07-26" sheetId="8" r:id="rId10"/>
+    <sheet name="new_2021-06-18" sheetId="12" r:id="rId6"/>
+    <sheet name="2021-06-21" sheetId="1" r:id="rId7"/>
+    <sheet name="2021-06-22" sheetId="2" r:id="rId8"/>
+    <sheet name="2021-07-13" sheetId="6" r:id="rId9"/>
+    <sheet name="2021-07-25" sheetId="7" r:id="rId10"/>
+    <sheet name="2021-07-26" sheetId="8" r:id="rId11"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="128">
   <si>
     <t>timestr</t>
   </si>
@@ -388,13 +389,46 @@
     <t>Dessau-Rosslau (13 UTC)</t>
   </si>
   <si>
-    <t>Cottbus (10:45 UTC)</t>
-  </si>
-  <si>
     <t>16:45 UTC</t>
   </si>
   <si>
     <t>16 UTC</t>
+  </si>
+  <si>
+    <t>2021-06-01 14:04:48</t>
+  </si>
+  <si>
+    <t>2021-06-01 14:00:32</t>
+  </si>
+  <si>
+    <t>2021-06-01 13:45:36</t>
+  </si>
+  <si>
+    <t>2021-06-01 13:28:32</t>
+  </si>
+  <si>
+    <t>2021-06-01 13:05:04</t>
+  </si>
+  <si>
+    <t>Cottbus (11:10 UTC)</t>
+  </si>
+  <si>
+    <t>2021-06-02 12:39:28</t>
+  </si>
+  <si>
+    <t>2021-06-02 11:50:24</t>
+  </si>
+  <si>
+    <t>2021-06-02 10:59:12</t>
+  </si>
+  <si>
+    <t>Vogesen (13:45 UTC)</t>
+  </si>
+  <si>
+    <t>2021-06-18 13:54:08</t>
+  </si>
+  <si>
+    <t>2021-06-18 14:04:48</t>
   </si>
 </sst>
 </file>
@@ -793,20 +827,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF23858F-1116-C34C-9921-DACE869774B7}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="21.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>113</v>
       </c>
       <c r="D1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -824,6 +861,91 @@
       </c>
       <c r="E2" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="C3" s="2">
+        <v>51.974820000000001</v>
+      </c>
+      <c r="D3" s="2">
+        <v>12.28229</v>
+      </c>
+      <c r="E3" s="2">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
+        <v>1408</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C4" s="2">
+        <v>51.862439999999999</v>
+      </c>
+      <c r="D4" s="2">
+        <v>12.41417</v>
+      </c>
+      <c r="E4" s="2">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="2">
+        <v>2432</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C5" s="2">
+        <v>51.733910000000002</v>
+      </c>
+      <c r="D5" s="2">
+        <v>12.420210000000001</v>
+      </c>
+      <c r="E5" s="2">
+        <v>875</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
+        <v>3328</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C6" s="2">
+        <v>51.677819999999997</v>
+      </c>
+      <c r="D6" s="2">
+        <v>12.46496</v>
+      </c>
+      <c r="E6" s="2">
+        <v>1144</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="2">
+        <v>3584</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C7" s="2">
+        <v>51.799379999999999</v>
+      </c>
+      <c r="D7" s="2">
+        <v>12.69952</v>
+      </c>
+      <c r="E7" s="2">
+        <v>1236</v>
       </c>
     </row>
   </sheetData>
@@ -832,6 +954,131 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A3968C7-932E-DE42-B8DB-FCDE033761CD}">
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="21.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>8960</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C3" s="2">
+        <v>52.604300000000002</v>
+      </c>
+      <c r="D3" s="2">
+        <v>13.40624</v>
+      </c>
+      <c r="E3" s="2">
+        <v>4718</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>9600</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C4" s="2">
+        <v>52.664369999999998</v>
+      </c>
+      <c r="D4" s="2">
+        <v>13.39208</v>
+      </c>
+      <c r="E4" s="2">
+        <v>5127</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>10496</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C5" s="2">
+        <v>52.778709999999997</v>
+      </c>
+      <c r="D5" s="2">
+        <v>13.45257</v>
+      </c>
+      <c r="E5" s="2">
+        <v>5613</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>11904</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C6" s="2">
+        <v>52.754660000000001</v>
+      </c>
+      <c r="D6" s="2">
+        <v>13.29097</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>12288</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C7" s="2">
+        <v>52.808070000000001</v>
+      </c>
+      <c r="D7" s="2">
+        <v>13.30294</v>
+      </c>
+      <c r="E7" s="2">
+        <v>6679</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7F7B32F-6924-6040-ACE3-BB1A6B58F40B}">
   <dimension ref="A1:E13"/>
   <sheetViews>
@@ -1019,20 +1266,91 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E29CFA6B-7352-4E46-AB60-955A801EFDF9}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="21.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C1" t="s">
         <v>114</v>
       </c>
-      <c r="C1" t="s">
-        <v>115</v>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="2">
+        <v>640</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C3" s="2">
+        <v>51.425780000000003</v>
+      </c>
+      <c r="D3" s="2">
+        <v>15.00122</v>
+      </c>
+      <c r="E3" s="2">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
+        <v>3712</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C4" s="2">
+        <v>51.779989999999998</v>
+      </c>
+      <c r="D4" s="2">
+        <v>14.82353</v>
+      </c>
+      <c r="E4" s="2">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="2">
+        <v>6656</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C5" s="2">
+        <v>51.873350000000002</v>
+      </c>
+      <c r="D5" s="2">
+        <v>14.818429999999999</v>
+      </c>
+      <c r="E5" s="2">
+        <v>740</v>
       </c>
     </row>
   </sheetData>
@@ -1879,7 +2197,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection sqref="A1:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2081,11 +2399,85 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BDE2DEE-A56D-B14A-BC57-695C8F6A27FF}">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="21.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="2">
+        <v>6528</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C3" s="2">
+        <v>48.134929999999997</v>
+      </c>
+      <c r="D3" s="2">
+        <v>7.1364470000000004</v>
+      </c>
+      <c r="E3" s="2">
+        <v>952</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
+        <v>7168</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="C4" s="2">
+        <v>48.249920000000003</v>
+      </c>
+      <c r="D4" s="2">
+        <v>7.1430720000000001</v>
+      </c>
+      <c r="E4" s="2">
+        <v>1071</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFFBE367-4360-B44F-9C43-4DE44BEC2FA8}">
   <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2364,7 +2756,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FA042F6-C877-5641-8DBA-45F8988DCF31}">
   <dimension ref="A1:E26"/>
   <sheetViews>
@@ -2754,7 +3146,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C7CD297-692E-FF45-8AAB-4B75C66A5DFB}">
   <dimension ref="A1:E8"/>
   <sheetViews>
@@ -2894,129 +3286,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A3968C7-932E-DE42-B8DB-FCDE033761CD}">
-  <dimension ref="A1:E7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="21.83203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>8960</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="C3" s="2">
-        <v>52.604300000000002</v>
-      </c>
-      <c r="D3" s="2">
-        <v>13.40624</v>
-      </c>
-      <c r="E3" s="2">
-        <v>4718</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>9600</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="C4" s="2">
-        <v>52.664369999999998</v>
-      </c>
-      <c r="D4" s="2">
-        <v>13.39208</v>
-      </c>
-      <c r="E4" s="2">
-        <v>5127</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>10496</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="C5" s="2">
-        <v>52.778709999999997</v>
-      </c>
-      <c r="D5" s="2">
-        <v>13.45257</v>
-      </c>
-      <c r="E5" s="2">
-        <v>5613</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>11904</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="C6" s="2">
-        <v>52.754660000000001</v>
-      </c>
-      <c r="D6" s="2">
-        <v>13.29097</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>12288</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="C7" s="2">
-        <v>52.808070000000001</v>
-      </c>
-      <c r="D7" s="2">
-        <v>13.30294</v>
-      </c>
-      <c r="E7" s="2">
-        <v>6679</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>